<commit_message>
AutoCommit_17 июня 2024 г. 10:13:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Сумма</t>
+  </si>
+  <si>
+    <t>изм</t>
   </si>
 </sst>
 </file>
@@ -555,13 +558,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -571,12 +574,12 @@
     <col min="3" max="10" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -605,7 +608,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -631,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -670,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -709,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -748,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -787,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -826,7 +829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -846,26 +849,29 @@
         <v>5</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M9" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -904,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -943,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -982,7 +988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 10:35:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -927,26 +927,29 @@
         <v>5</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="M11" s="8">
         <v>3</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 11:07:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>изм</t>
+  </si>
+  <si>
+    <t>BPV</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1245,26 +1248,29 @@
         <v>5</v>
       </c>
       <c r="G19" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H19" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I19" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M19" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1401,26 +1407,29 @@
         <v>5</v>
       </c>
       <c r="G23" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H23" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I23" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J23" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M23" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 11:12:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>BPV</t>
+  </si>
+  <si>
+    <t>HJHFJKR</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
+      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1644,23 +1647,26 @@
         <v>5</v>
       </c>
       <c r="G29" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H29" s="5">
         <v>5</v>
       </c>
       <c r="I29" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J29" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="M29" s="8">
         <v>4</v>
+      </c>
+      <c r="O29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 11:15:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -570,7 +570,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -816,23 +816,26 @@
         <v>5</v>
       </c>
       <c r="G8" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="M8" s="8">
         <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 20:12:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>2ИСИП-822: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>аываыв</t>
+  </si>
+  <si>
+    <t>Расставить двойки</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -618,6 +621,9 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 20:21:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -170,7 +170,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -266,6 +272,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -576,7 +592,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -624,11 +640,21 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="1"/>
@@ -653,20 +679,20 @@
         <v>5</v>
       </c>
       <c r="G4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <f>SUM(C4:J4)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M4" s="8">
         <v>3</v>
@@ -770,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5">
         <v>5</v>
@@ -783,7 +809,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M7" s="8">
         <v>4</v>
@@ -797,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -822,7 +848,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M8" s="8">
         <v>3</v>
@@ -893,20 +919,20 @@
         <v>5</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M10" s="8">
         <v>3</v>
@@ -1013,20 +1039,20 @@
         <v>5</v>
       </c>
       <c r="G13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M13" s="8">
         <v>3</v>
@@ -1094,20 +1120,20 @@
         <v>5</v>
       </c>
       <c r="G15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M15" s="8">
         <v>3</v>
@@ -1178,14 +1204,14 @@
         <v>5</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M17" s="8">
         <v>4</v>
@@ -1211,20 +1237,20 @@
         <v>5</v>
       </c>
       <c r="G18" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M18" s="8">
         <v>3</v>
@@ -1331,20 +1357,20 @@
         <v>5</v>
       </c>
       <c r="G21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M21" s="8">
         <v>3</v>
@@ -1439,32 +1465,33 @@
         <v>21</v>
       </c>
       <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0</v>
-      </c>
-      <c r="I24" s="7">
-        <v>0</v>
-      </c>
-      <c r="J24" s="4">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>2</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2</v>
+      </c>
+      <c r="H24" s="10">
+        <v>2</v>
+      </c>
+      <c r="I24" s="11">
+        <v>2</v>
+      </c>
+      <c r="J24" s="9">
+        <v>2</v>
+      </c>
+      <c r="K24" s="12"/>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M24" s="8">
         <v>3</v>
@@ -1490,20 +1517,20 @@
         <v>5</v>
       </c>
       <c r="G25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M25" s="8">
         <v>3</v>
@@ -1676,7 +1703,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="4">
         <v>5</v>
@@ -1691,17 +1718,17 @@
         <v>5</v>
       </c>
       <c r="H30" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="M30" s="8">
         <v>3</v>
@@ -1775,11 +1802,11 @@
         <v>5</v>
       </c>
       <c r="J32" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M32" s="8">
         <v>4</v>
@@ -1814,11 +1841,11 @@
         <v>5</v>
       </c>
       <c r="J33" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M33" s="8">
         <v>4</v>
@@ -1853,11 +1880,11 @@
         <v>5</v>
       </c>
       <c r="J34" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L34">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M34" s="8">
         <v>4</v>
@@ -1892,11 +1919,11 @@
         <v>5</v>
       </c>
       <c r="J35" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M35" s="8">
         <v>4</v>
@@ -1931,11 +1958,11 @@
         <v>5</v>
       </c>
       <c r="J36" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M36" s="8">
         <v>4</v>
@@ -1970,11 +1997,11 @@
         <v>5</v>
       </c>
       <c r="J37" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M37" s="8">
         <v>4</v>
@@ -2009,11 +2036,11 @@
         <v>5</v>
       </c>
       <c r="J38" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M38" s="8">
         <v>4</v>
@@ -2048,11 +2075,11 @@
         <v>5</v>
       </c>
       <c r="J39" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M39" s="8">
         <v>4</v>
@@ -2087,11 +2114,11 @@
         <v>5</v>
       </c>
       <c r="J40" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L40">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M40" s="8">
         <v>4</v>
@@ -2126,11 +2153,11 @@
         <v>5</v>
       </c>
       <c r="J41" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M41" s="8">
         <v>4</v>
@@ -2165,11 +2192,11 @@
         <v>5</v>
       </c>
       <c r="J42" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M42" s="8">
         <v>4</v>
@@ -2204,11 +2231,11 @@
         <v>5</v>
       </c>
       <c r="J43" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M43" s="8">
         <v>4</v>
@@ -2243,11 +2270,11 @@
         <v>5</v>
       </c>
       <c r="J44" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M44" s="8">
         <v>4</v>
@@ -2282,11 +2309,11 @@
         <v>5</v>
       </c>
       <c r="J45" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M45" s="8">
         <v>4</v>
@@ -2321,11 +2348,11 @@
         <v>5</v>
       </c>
       <c r="J46" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L46">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M46" s="8">
         <v>4</v>
@@ -2360,11 +2387,11 @@
         <v>5</v>
       </c>
       <c r="J47" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M47" s="8">
         <v>4</v>
@@ -2399,11 +2426,11 @@
         <v>5</v>
       </c>
       <c r="J48" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M48" s="8">
         <v>4</v>
@@ -2438,11 +2465,11 @@
         <v>5</v>
       </c>
       <c r="J49" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M49" s="8">
         <v>4</v>
@@ -2477,11 +2504,11 @@
         <v>5</v>
       </c>
       <c r="J50" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M50" s="8">
         <v>4</v>
@@ -2492,7 +2519,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="C4:J50 M4:M51">
+  <conditionalFormatting sqref="C4:J23 M4:M51 C25:J50 C24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 20:35:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -589,10 +589,10 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -655,9 +655,15 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="1"/>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 16:29:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-822_ТерВер.xlsx
+++ b/2ИСИП-822_ТерВер.xlsx
@@ -580,10 +580,10 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="O6:O48"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -913,23 +913,23 @@
         <v>5</v>
       </c>
       <c r="G10" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J10" s="4">
         <v>2</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="M10" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1342,10 +1342,10 @@
         <v>5</v>
       </c>
       <c r="G21" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H21" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I21" s="7">
         <v>2</v>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="M21" s="8">
         <v>4</v>

</xml_diff>